<commit_message>
finished making the 2024 map for endurance lol. took forever
</commit_message>
<xml_diff>
--- a/2024 MI Endurance map.xlsx
+++ b/2024 MI Endurance map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stuff\repos\endurance_sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BD732F7-85C4-4F77-BA9E-35579C7F93EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DD82C6-A15D-4210-A589-2FF91304F08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB74DD3E-02BD-46F0-859D-014F0E163676}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{BB74DD3E-02BD-46F0-859D-014F0E163676}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="6">
   <si>
     <t>turn type</t>
   </si>
@@ -69,12 +69,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -89,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -106,6 +113,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{509884BB-803F-4F28-B2A5-9DDD90E3073B}" name="Table1" displayName="Table1" ref="A1:C82" totalsRowShown="0">
+  <autoFilter ref="A1:C82" xr:uid="{509884BB-803F-4F28-B2A5-9DDD90E3073B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{67C43A36-6A94-4900-AAAF-D3F747EBD2EF}" name="turn type"/>
+    <tableColumn id="2" xr3:uid="{68BE3E73-7CA5-4F91-81BB-D0FF5EC07378}" name="section length"/>
+    <tableColumn id="3" xr3:uid="{5EE5AF67-4380-4AD7-968F-CEC9C33C0C13}" name="corner radius"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -425,13 +444,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C37A67-D37C-4B4B-BFD2-C0EA1667F1E8}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -629,7 +653,619 @@
         <v>29.672999999999998</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>19.056999999999999</v>
+      </c>
+      <c r="C21">
+        <v>16.45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>9.1720000000000006</v>
+      </c>
+      <c r="C22">
+        <v>9.1820000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>9.9350000000000005</v>
+      </c>
+      <c r="C23">
+        <v>6.7380000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>31.152999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>6.1020000000000003</v>
+      </c>
+      <c r="C25">
+        <v>10.048</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>10.757999999999999</v>
+      </c>
+      <c r="C26">
+        <v>10.704000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>8.7110000000000003</v>
+      </c>
+      <c r="C27">
+        <v>7.3150000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>9.3469999999999995</v>
+      </c>
+      <c r="C28">
+        <v>6.4960000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>3.948</v>
+      </c>
+      <c r="C29">
+        <v>4.5709999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>12.912000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>3.391</v>
+      </c>
+      <c r="C31">
+        <v>10.675000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>7.4859999999999998</v>
+      </c>
+      <c r="C32">
+        <v>26.28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>41.18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>6.875</v>
+      </c>
+      <c r="C34">
+        <v>18.981000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>13.268000000000001</v>
+      </c>
+      <c r="C35">
+        <v>16.884</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>10.564</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>7.2779999999999996</v>
+      </c>
+      <c r="C37">
+        <v>8.4870000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>14.798999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <v>21.731999999999999</v>
+      </c>
+      <c r="C39">
+        <v>29.079000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>25.72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>6.3579999999999997</v>
+      </c>
+      <c r="C41">
+        <v>17.177</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>6.0789999999999997</v>
+      </c>
+      <c r="C42">
+        <v>3.5110000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>6.923</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>6.0449999999999999</v>
+      </c>
+      <c r="C44">
+        <v>5.1449999999999996</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45">
+        <v>11.471</v>
+      </c>
+      <c r="C45">
+        <v>14.598000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <v>5.9930000000000003</v>
+      </c>
+      <c r="C46">
+        <v>3.996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47">
+        <v>9.4369999999999994</v>
+      </c>
+      <c r="C47">
+        <v>23.448</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48">
+        <v>15.106999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <v>7.3520000000000003</v>
+      </c>
+      <c r="C49">
+        <v>6.9180000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50">
+        <v>11.162000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>3.794</v>
+      </c>
+      <c r="C51">
+        <v>3.4540000000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52">
+        <v>5.7830000000000004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="1">
+        <v>3.2919999999999998</v>
+      </c>
+      <c r="C53" s="1">
+        <v>7.476</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>0.99</v>
+      </c>
+      <c r="C54">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55">
+        <v>44.55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>13.157999999999999</v>
+      </c>
+      <c r="C56">
+        <v>78.266000000000005</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57">
+        <v>13.127000000000001</v>
+      </c>
+      <c r="C57">
+        <v>83.661000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58">
+        <v>4.3920000000000003</v>
+      </c>
+      <c r="C58">
+        <v>5.1470000000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59">
+        <v>4.6289999999999996</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60">
+        <v>29.006</v>
+      </c>
+      <c r="C60">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>9.9930000000000003</v>
+      </c>
+      <c r="C61">
+        <v>11.56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62">
+        <v>10.685</v>
+      </c>
+      <c r="C62">
+        <v>11.656000000000001</v>
+      </c>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63">
+        <v>9.3989999999999991</v>
+      </c>
+      <c r="C63">
+        <v>14.19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="1">
+        <v>8.2780000000000005</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65">
+        <v>9.1869999999999994</v>
+      </c>
+      <c r="C65">
+        <v>13.676</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66">
+        <v>29.265999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67">
+        <v>15.781000000000001</v>
+      </c>
+      <c r="C67">
+        <v>14.955</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>24.922000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69">
+        <v>19.969000000000001</v>
+      </c>
+      <c r="C69">
+        <v>18.138999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70">
+        <v>28.196000000000002</v>
+      </c>
+      <c r="C70">
+        <v>49.97</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71">
+        <v>58.134999999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72">
+        <v>11.145</v>
+      </c>
+      <c r="C72">
+        <v>28.306999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73">
+        <v>11.922000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74">
+        <v>6.8579999999999997</v>
+      </c>
+      <c r="C74">
+        <v>8.5210000000000008</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75">
+        <v>17.893999999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76">
+        <v>5.7859999999999996</v>
+      </c>
+      <c r="C76">
+        <v>6.2549999999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77">
+        <v>16.988</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78">
+        <v>7.3419999999999996</v>
+      </c>
+      <c r="C78">
+        <v>7.6790000000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79">
+        <v>11.909000000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>4</v>
+      </c>
+      <c r="B80">
+        <v>12.116</v>
+      </c>
+      <c r="C80">
+        <v>10.33</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81">
+        <v>4.8040000000000003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ok updated the track to match the picture. i had messed up previously. still an error
i think the scale is off. i think it is 7.65m per square not 7.625. idk, the track is just slightly off now. but there are a couple corners that are a good bit off. not sure what i'll do, this is a much bigger time sink than expected :(
</commit_message>
<xml_diff>
--- a/2024 MI Endurance map.xlsx
+++ b/2024 MI Endurance map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stuff\repos\endurance_sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DD82C6-A15D-4210-A589-2FF91304F08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913B0EDA-3060-4768-865B-46158801655C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{BB74DD3E-02BD-46F0-859D-014F0E163676}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB74DD3E-02BD-46F0-859D-014F0E163676}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="7">
   <si>
     <t>turn type</t>
   </si>
@@ -55,12 +55,15 @@
   <si>
     <t>left</t>
   </si>
+  <si>
+    <t>Notes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,8 +71,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -79,6 +88,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -95,9 +110,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -116,12 +134,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{509884BB-803F-4F28-B2A5-9DDD90E3073B}" name="Table1" displayName="Table1" ref="A1:C82" totalsRowShown="0">
-  <autoFilter ref="A1:C82" xr:uid="{509884BB-803F-4F28-B2A5-9DDD90E3073B}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{509884BB-803F-4F28-B2A5-9DDD90E3073B}" name="Table1" displayName="Table1" ref="A1:D85" totalsRowShown="0">
+  <autoFilter ref="A1:D85" xr:uid="{509884BB-803F-4F28-B2A5-9DDD90E3073B}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{67C43A36-6A94-4900-AAAF-D3F747EBD2EF}" name="turn type"/>
     <tableColumn id="2" xr3:uid="{68BE3E73-7CA5-4F91-81BB-D0FF5EC07378}" name="section length"/>
     <tableColumn id="3" xr3:uid="{5EE5AF67-4380-4AD7-968F-CEC9C33C0C13}" name="corner radius"/>
+    <tableColumn id="4" xr3:uid="{1863D0FC-762E-47CC-BE6B-4037949B54C7}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -444,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C37A67-D37C-4B4B-BFD2-C0EA1667F1E8}">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +476,7 @@
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,8 +486,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -476,7 +498,7 @@
         <v>11.593</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -487,7 +509,7 @@
         <v>5.819</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -495,26 +517,26 @@
         <v>8.9909999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>5.3280000000000003</v>
-      </c>
-      <c r="C5">
-        <v>4.2290000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>5.327</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4.2240000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
-        <v>10.071</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>10.065</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -525,7 +547,7 @@
         <v>4.2969999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -533,156 +555,156 @@
         <v>12.91</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
         <v>7.5540000000000003</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>7.0030000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10">
+    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4">
         <v>13.429</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11">
+    <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2">
         <v>4.8380000000000001</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>4.6310000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12">
+    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2">
         <v>9.2579999999999991</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13">
+    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2">
         <v>4.7050000000000001</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>4.6050000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14">
+    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2">
         <v>13.417999999999999</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>13.321</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15">
+    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2">
         <v>8.1920000000000002</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>7.4530000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16">
+    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2">
         <v>4.6150000000000002</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>8.5389999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17">
+    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2">
         <v>5.782</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18">
+    <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2">
         <v>25.154</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19">
+    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="2">
         <v>10.106</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>10.281000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20">
+    <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="2">
         <v>4.8079999999999998</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>29.672999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21">
+    <row r="21" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2">
         <v>19.056999999999999</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>16.45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22">
+    <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="2">
         <v>9.1720000000000006</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>9.1820000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23">
+    <row r="23" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1">
         <v>9.9350000000000005</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>6.7380000000000004</v>
       </c>
     </row>
@@ -784,7 +806,7 @@
         <v>3</v>
       </c>
       <c r="B33">
-        <v>41.18</v>
+        <v>41.618000000000002</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -792,10 +814,10 @@
         <v>5</v>
       </c>
       <c r="B34">
-        <v>6.875</v>
+        <v>3.2109999999999999</v>
       </c>
       <c r="C34">
-        <v>18.981000000000002</v>
+        <v>6.7990000000000004</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -803,10 +825,10 @@
         <v>4</v>
       </c>
       <c r="B35">
-        <v>13.268000000000001</v>
+        <v>1.4430000000000001</v>
       </c>
       <c r="C35">
-        <v>16.884</v>
+        <v>3.1709999999999998</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -814,7 +836,7 @@
         <v>3</v>
       </c>
       <c r="B36">
-        <v>10.564</v>
+        <v>23.812999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -822,48 +844,48 @@
         <v>5</v>
       </c>
       <c r="B37">
-        <v>7.2779999999999996</v>
+        <v>6.875</v>
       </c>
       <c r="C37">
-        <v>8.4870000000000001</v>
+        <v>18.981000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B38">
-        <v>14.798999999999999</v>
+        <v>13.268000000000001</v>
+      </c>
+      <c r="C38">
+        <v>16.884</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B39">
-        <v>21.731999999999999</v>
-      </c>
-      <c r="C39">
-        <v>29.079000000000001</v>
+        <v>10.564</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B40">
-        <v>25.72</v>
+        <v>7.2779999999999996</v>
+      </c>
+      <c r="C40">
+        <v>8.4870000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B41">
-        <v>6.3579999999999997</v>
-      </c>
-      <c r="C41">
-        <v>17.177</v>
+        <v>14.798999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -871,10 +893,10 @@
         <v>4</v>
       </c>
       <c r="B42">
-        <v>6.0789999999999997</v>
+        <v>21.731999999999999</v>
       </c>
       <c r="C42">
-        <v>3.5110000000000001</v>
+        <v>29.079000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -882,7 +904,7 @@
         <v>3</v>
       </c>
       <c r="B43">
-        <v>6.923</v>
+        <v>25.72</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -890,10 +912,10 @@
         <v>5</v>
       </c>
       <c r="B44">
-        <v>6.0449999999999999</v>
+        <v>6.3579999999999997</v>
       </c>
       <c r="C44">
-        <v>5.1449999999999996</v>
+        <v>17.177</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -901,364 +923,394 @@
         <v>4</v>
       </c>
       <c r="B45">
-        <v>11.471</v>
+        <v>6.0789999999999997</v>
       </c>
       <c r="C45">
-        <v>14.598000000000001</v>
+        <v>3.5110000000000001</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B46">
-        <v>5.9930000000000003</v>
-      </c>
-      <c r="C46">
-        <v>3.996</v>
+        <v>6.923</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B47">
-        <v>9.4369999999999994</v>
+        <v>6.0449999999999999</v>
       </c>
       <c r="C47">
-        <v>23.448</v>
+        <v>5.1449999999999996</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B48">
+        <v>11.471</v>
+      </c>
+      <c r="C48">
+        <v>14.598000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <v>5.9930000000000003</v>
+      </c>
+      <c r="C49">
+        <v>3.996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50">
+        <v>9.4369999999999994</v>
+      </c>
+      <c r="C50">
+        <v>23.448</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51">
         <v>15.106999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>4</v>
-      </c>
-      <c r="B49">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52">
         <v>7.3520000000000003</v>
       </c>
-      <c r="C49">
+      <c r="C52">
         <v>6.9180000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53">
         <v>11.162000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54">
         <v>3.794</v>
       </c>
-      <c r="C51">
+      <c r="C54">
         <v>3.4540000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>3</v>
-      </c>
-      <c r="B52">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55">
         <v>5.7830000000000004</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B53" s="1">
+    <row r="56" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="2">
         <v>3.2919999999999998</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C56" s="2">
         <v>7.476</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57">
         <v>0.99</v>
       </c>
-      <c r="C54">
+      <c r="C57">
         <v>2.33</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>3</v>
-      </c>
-      <c r="B55">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58">
         <v>44.55</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>5</v>
-      </c>
-      <c r="B56">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59">
         <v>13.157999999999999</v>
       </c>
-      <c r="C56">
+      <c r="C59">
         <v>78.266000000000005</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>4</v>
-      </c>
-      <c r="B57">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60">
         <v>13.127000000000001</v>
       </c>
-      <c r="C57">
+      <c r="C60">
         <v>83.661000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61">
         <v>4.3920000000000003</v>
       </c>
-      <c r="C58">
+      <c r="C61">
         <v>5.1470000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>3</v>
-      </c>
-      <c r="B59">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62">
         <v>4.6289999999999996</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>4</v>
-      </c>
-      <c r="B60">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63">
         <v>29.006</v>
       </c>
-      <c r="C60">
+      <c r="C63">
         <v>22.7</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>5</v>
-      </c>
-      <c r="B61">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64">
         <v>9.9930000000000003</v>
       </c>
-      <c r="C61">
+      <c r="C64">
         <v>11.56</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>4</v>
-      </c>
-      <c r="B62">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65">
         <v>10.685</v>
       </c>
-      <c r="C62">
+      <c r="C65">
         <v>11.656000000000001</v>
       </c>
-      <c r="E62" s="1"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63">
+      <c r="E65" s="2"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66">
         <v>9.3989999999999991</v>
       </c>
-      <c r="C63">
+      <c r="C66">
         <v>14.19</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B64" s="1">
+    <row r="67" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" s="1">
         <v>8.2780000000000005</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>4</v>
-      </c>
-      <c r="B65">
+    <row r="68" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" s="1">
         <v>9.1869999999999994</v>
       </c>
-      <c r="C65">
+      <c r="C68" s="3">
         <v>13.676</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>3</v>
-      </c>
-      <c r="B66">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69">
         <v>29.265999999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>5</v>
-      </c>
-      <c r="B67">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70">
         <v>15.781000000000001</v>
       </c>
-      <c r="C67">
+      <c r="C70">
         <v>14.955</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>3</v>
-      </c>
-      <c r="B68">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71">
         <v>24.922000000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>4</v>
-      </c>
-      <c r="B69">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72">
         <v>19.969000000000001</v>
       </c>
-      <c r="C69">
+      <c r="C72">
         <v>18.138999999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>5</v>
-      </c>
-      <c r="B70">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73">
         <v>28.196000000000002</v>
       </c>
-      <c r="C70">
+      <c r="C73">
         <v>49.97</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>3</v>
-      </c>
-      <c r="B71">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74">
         <v>58.134999999999998</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>5</v>
-      </c>
-      <c r="B72">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75">
         <v>11.145</v>
       </c>
-      <c r="C72">
+      <c r="C75">
         <v>28.306999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>3</v>
-      </c>
-      <c r="B73">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76">
         <v>11.922000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>4</v>
-      </c>
-      <c r="B74">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77">
         <v>6.8579999999999997</v>
       </c>
-      <c r="C74">
+      <c r="C77">
         <v>8.5210000000000008</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>3</v>
-      </c>
-      <c r="B75">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78">
         <v>17.893999999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>5</v>
-      </c>
-      <c r="B76">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79">
         <v>5.7859999999999996</v>
       </c>
-      <c r="C76">
+      <c r="C79">
         <v>6.2549999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>3</v>
-      </c>
-      <c r="B77">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80">
         <v>16.988</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>4</v>
-      </c>
-      <c r="B78">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>4</v>
+      </c>
+      <c r="B81">
         <v>7.3419999999999996</v>
       </c>
-      <c r="C78">
+      <c r="C81">
         <v>7.6790000000000003</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>3</v>
-      </c>
-      <c r="B79">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82">
         <v>11.909000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>4</v>
-      </c>
-      <c r="B80">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>4</v>
+      </c>
+      <c r="B83">
         <v>12.116</v>
       </c>
-      <c r="C80">
+      <c r="C83">
         <v>10.33</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>3</v>
-      </c>
-      <c r="B81">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84">
         <v>4.8040000000000003</v>
       </c>
     </row>

</xml_diff>